<commit_message>
Code till 29th may
</commit_message>
<xml_diff>
--- a/src/main/resources/ExcelData.xlsx
+++ b/src/main/resources/ExcelData.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\eclipse-workspace\QALegendBilling\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A26643-06DE-4243-BB8F-E9B6BC66025D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0711290E-1FF6-4BF3-8391-86784C6E8C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
+    <sheet name="SearchUser" sheetId="4" r:id="rId2"/>
+    <sheet name="MailReset" sheetId="2" r:id="rId3"/>
+    <sheet name="InvalidLoginData" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>UserName</t>
   </si>
@@ -34,16 +37,39 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>ad</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>aswa@gmail.com</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>ljhg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -66,13 +92,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -353,13 +382,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -381,4 +410,103 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8042F748-8567-436A-B450-FBDFE9C5C9EB}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>123456</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7CA4DAF-090B-4B81-A759-64C14CCC8EF3}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{8CD0C857-A65F-48D1-B8C7-7931EAA84E3C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89972E9B-8C1B-4EB5-B491-8F7F7901377D}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>123456</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>